<commit_message>
update readme file and add demo2
</commit_message>
<xml_diff>
--- a/usePython/outs/demo1/4633087/4633087-texts.xlsx
+++ b/usePython/outs/demo1/4633087/4633087-texts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>MappingID</t>
   </si>
@@ -49,22 +49,25 @@
     <t>356.25</t>
   </si>
   <si>
+    <t>#fbfbfb</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
+  </si>
+  <si>
+    <t>#fdfdfd</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>328.98</t>
+  </si>
+  <si>
     <t>#fefefe</t>
-  </si>
-  <si>
-    <t>#fafafa</t>
-  </si>
-  <si>
-    <t>#fdfdfd</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>FRIDAY</t>
-  </si>
-  <si>
-    <t>328.98</t>
   </si>
   <si>
     <t>#fcd602</t>
@@ -125,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +154,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF040404"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF020202"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF010101"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,20 +182,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF050505"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF020202"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF0329FD"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,19 +246,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFBFBFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDFDFD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFEFEFE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFAFAFA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDFDFD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -330,6 +346,7 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,80 +716,80 @@
       <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>23</v>
+      <c r="G4" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>29</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>34</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>